<commit_message>
remove benchmark to separate project, updated results
</commit_message>
<xml_diff>
--- a/etc/doc/Benchmarks.xlsx
+++ b/etc/doc/Benchmarks.xlsx
@@ -4,23 +4,22 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="24120" windowHeight="12360" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="24120" windowHeight="12360" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="BeanUtil" sheetId="1" r:id="rId1"/>
-    <sheet name="Proxetta" sheetId="2" r:id="rId2"/>
+    <sheet name="Mutable" sheetId="5" r:id="rId2"/>
     <sheet name="JDateTime" sheetId="3" r:id="rId3"/>
-    <sheet name="Sorting" sheetId="4" r:id="rId4"/>
-    <sheet name="Mutable" sheetId="5" r:id="rId5"/>
-    <sheet name="Base64" sheetId="6" r:id="rId6"/>
-    <sheet name="StringBand" sheetId="7" r:id="rId7"/>
+    <sheet name="Proxetta" sheetId="2" r:id="rId4"/>
+    <sheet name="Base64" sheetId="6" r:id="rId5"/>
+    <sheet name="StringBand" sheetId="7" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="20">
   <si>
     <t>test #1</t>
   </si>
@@ -34,28 +33,13 @@
     <t>method invocation</t>
   </si>
   <si>
-    <t>dynaop (cglib)</t>
-  </si>
-  <si>
     <t>calendar</t>
-  </si>
-  <si>
-    <t>jodd merge</t>
-  </si>
-  <si>
-    <t>jodd quick</t>
-  </si>
-  <si>
-    <t>java</t>
   </si>
   <si>
     <t>integer</t>
   </si>
   <si>
     <t>Sun</t>
-  </si>
-  <si>
-    <t>test #3</t>
   </si>
   <si>
     <t>Harder</t>
@@ -73,31 +57,44 @@
     <t>StringBuilder</t>
   </si>
   <si>
-    <t>10^4</t>
-  </si>
-  <si>
-    <t>10^2</t>
-  </si>
-  <si>
-    <t>10^3</t>
-  </si>
-  <si>
-    <t>10^5</t>
-  </si>
-  <si>
     <t>StringBand</t>
   </si>
   <si>
-    <t>StringBand
-(w prediction)</t>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>sd</t>
+  </si>
+  <si>
+    <t>cglib</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>add2</t>
+  </si>
+  <si>
+    <t>add3</t>
+  </si>
+  <si>
+    <t>add5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -125,13 +122,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -174,7 +181,7 @@
               <a:rPr lang="sr-Latn-CS" baseline="0">
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>BeanUtil performance</a:t>
+              <a:t>BeanUtil benchmark</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" baseline="0">
               <a:latin typeface="+mn-lt"/>
@@ -207,9 +214,44 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>BeanUtil!$C$3:$C$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>23.088000000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>86.784000000000006</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>BeanUtil!$C$3:$C$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>23.088000000000001</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>86.784000000000006</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>BeanUtil!$A$2:$A$3</c:f>
+              <c:f>BeanUtil!$A$3:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -223,15 +265,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BeanUtil!$D$2:$D$3</c:f>
+              <c:f>BeanUtil!$B$3:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>2091</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>6205</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -242,7 +284,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>BeanUtil!$C$1</c:f>
+              <c:f>BeanUtil!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -259,9 +301,44 @@
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>BeanUtil!$E$3:$E$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>9.3529999999999998</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>43.354999999999997</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>BeanUtil!$E$3:$E$4</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>9.3529999999999998</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>43.354999999999997</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>BeanUtil!$A$2:$A$3</c:f>
+              <c:f>BeanUtil!$A$3:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -275,15 +352,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>BeanUtil!$E$2:$E$3</c:f>
+              <c:f>BeanUtil!$D$3:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>35.117511207716348</c:v>
+                  <c:v>1058</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.862519752909066</c:v>
+                  <c:v>3083</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -299,11 +376,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="57261568"/>
-        <c:axId val="104254272"/>
+        <c:axId val="42835456"/>
+        <c:axId val="124994112"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="57261568"/>
+        <c:axId val="42835456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -312,7 +389,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104254272"/>
+        <c:crossAx val="124994112"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -320,10 +397,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104254272"/>
+        <c:axId val="124994112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -339,7 +415,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="sr-Latn-CS" sz="1100" baseline="0"/>
-                  <a:t>Time [%]</a:t>
+                  <a:t>Time [ms]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -351,10 +427,9 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="57261568"/>
+        <c:crossAx val="42835456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="20"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -413,10 +488,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
+      <c14:style val="134"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="2"/>
+      <c:style val="34"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -430,14 +505,25 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="sr-Latn-CS"/>
-              <a:t>Proxetta performance</a:t>
+              <a:rPr lang="sr-Latn-CS" baseline="0">
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Mutable Numbers benchmark</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" baseline="0">
+              <a:latin typeface="+mn-lt"/>
+            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18732935719019217"/>
+          <c:y val="2.8596961572832886E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -452,35 +538,64 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Proxetta!$B$1</c:f>
+              <c:f>Mutable!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>dynaop (cglib)</c:v>
+                  <c:v>integer</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Mutable!$C$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>16.646000000000001</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Mutable!$C$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>16.646000000000001</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Proxetta!$A$2</c:f>
+              <c:f>Mutable!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>method invocation</c:v>
+                  <c:v>test #1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Proxetta!$D$2</c:f>
+              <c:f>Mutable!$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>813.19399999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -491,7 +606,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Proxetta!$C$1</c:f>
+              <c:f>Mutable!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -508,25 +623,54 @@
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Mutable!$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>23.797000000000001</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Mutable!$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>23.797000000000001</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Proxetta!$A$2</c:f>
+              <c:f>Mutable!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>method invocation</c:v>
+                  <c:v>test #1</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Proxetta!$E$2</c:f>
+              <c:f>Mutable!$D$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>24.44342367171949</c:v>
+                  <c:v>170.78800000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -541,32 +685,13 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="75"/>
-        <c:overlap val="40"/>
-        <c:axId val="59561984"/>
-        <c:axId val="104256576"/>
+        <c:axId val="42834944"/>
+        <c:axId val="124996416"/>
       </c:barChart>
-      <c:catAx>
-        <c:axId val="59561984"/>
+      <c:valAx>
+        <c:axId val="124996416"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104256576"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="104256576"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -581,35 +706,41 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="sr-Latn-CS" sz="1200" baseline="0"/>
-                  <a:t>Time [%]</a:t>
+                  <a:rPr lang="sr-Latn-CS" sz="1100" baseline="0"/>
+                  <a:t>Time [ms]</a:t>
                 </a:r>
-                <a:endParaRPr lang="en-US" sz="1200" baseline="0"/>
               </a:p>
             </c:rich>
           </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="42834944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:catAx>
+        <c:axId val="42834944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-        </c:spPr>
-        <c:crossAx val="59561984"/>
+        <c:crossAx val="124996416"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="20"/>
-      </c:valAx>
-      <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="bg1">
-            <a:lumMod val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </c:spPr>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
@@ -620,29 +751,20 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="1200" b="1" i="0" baseline="0"/>
+              <a:defRPr sz="1200" b="1"/>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
       </c:legendEntry>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.73570822397200364"/>
-          <c:y val="0.16755043013391041"/>
-          <c:w val="0.24484733158355226"/>
-          <c:h val="0.15488984556817095"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200" baseline="0"/>
+            <a:defRPr sz="1200"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -652,14 +774,9 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
+    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -692,7 +809,7 @@
               <a:rPr lang="sr-Latn-CS" baseline="0">
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>JDateTime performance</a:t>
+              <a:t>JDateTime benchmark</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" baseline="0">
               <a:latin typeface="+mn-lt"/>
@@ -725,9 +842,44 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(JDateTime!$C$3,JDateTime!$C$4)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>340</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>385</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(JDateTime!$C$3,JDateTime!$C$4)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>340</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>385</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>JDateTime!$A$2:$A$3</c:f>
+              <c:f>JDateTime!$A$3:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -741,15 +893,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>JDateTime!$D$2:$D$3</c:f>
+              <c:f>JDateTime!$B$3:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>12260</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>8205</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -760,7 +912,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>JDateTime!$C$1</c:f>
+              <c:f>JDateTime!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -777,9 +929,44 @@
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>(JDateTime!$E$3,JDateTime!$E$4)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>234</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>179</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>(JDateTime!$E$3,JDateTime!$E$4)</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>234</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>179</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>JDateTime!$A$2:$A$3</c:f>
+              <c:f>JDateTime!$A$3:$A$4</c:f>
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
@@ -793,15 +980,15 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>JDateTime!$E$2:$E$3</c:f>
+              <c:f>JDateTime!$D$3:$D$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>57.187845774108439</c:v>
+                  <c:v>6617</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>46.583028955587316</c:v>
+                  <c:v>4092</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -817,11 +1004,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="59518976"/>
-        <c:axId val="104258880"/>
+        <c:axId val="126910464"/>
+        <c:axId val="124998720"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="59518976"/>
+        <c:axId val="126910464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -830,7 +1017,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="104258880"/>
+        <c:crossAx val="124998720"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -838,10 +1025,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="104258880"/>
+        <c:axId val="124998720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -857,7 +1043,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="sr-Latn-CS" sz="1100" baseline="0"/>
-                  <a:t>Time [%]</a:t>
+                  <a:t>Time [ms]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -869,10 +1055,9 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59518976"/>
+        <c:crossAx val="126910464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="20"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -931,10 +1116,10 @@
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="134"/>
+      <c14:style val="102"/>
     </mc:Choice>
     <mc:Fallback>
-      <c:style val="34"/>
+      <c:style val="2"/>
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
@@ -948,14 +1133,10 @@
               <a:defRPr/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="sr-Latn-CS" baseline="0">
-                <a:latin typeface="+mn-lt"/>
-              </a:rPr>
-              <a:t>Sorting performance</a:t>
+              <a:rPr lang="sr-Latn-CS"/>
+              <a:t>Proxetta benchmark</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" baseline="0">
-              <a:latin typeface="+mn-lt"/>
-            </a:endParaRPr>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -974,35 +1155,67 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sorting!$B$1</c:f>
+              <c:f>Proxetta!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>java</c:v>
+                  <c:v>cglib</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:ln w="12700"/>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Proxetta!$C$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>274</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Proxetta!$C$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>274</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sorting!$A$2</c:f>
+              <c:f>Proxetta!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>test #1</c:v>
+                  <c:v>method invocation</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sorting!$E$2</c:f>
+              <c:f>Proxetta!$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>5594</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1013,11 +1226,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sorting!$C$1</c:f>
+              <c:f>Proxetta!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>jodd merge</c:v>
+                  <c:v>jodd</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1030,25 +1243,54 @@
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Proxetta!$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>203</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Proxetta!$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>203</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Sorting!$A$2</c:f>
+              <c:f>Proxetta!$A$3</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>test #1</c:v>
+                  <c:v>method invocation</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sorting!$F$2</c:f>
+              <c:f>Proxetta!$D$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>57.152801949182042</c:v>
+                  <c:v>4260</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1064,11 +1306,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="59521024"/>
-        <c:axId val="39798464"/>
+        <c:axId val="125142016"/>
+        <c:axId val="125001024"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="59521024"/>
+        <c:axId val="125142016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1077,7 +1319,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39798464"/>
+        <c:crossAx val="125001024"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1085,10 +1327,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39798464"/>
+        <c:axId val="125001024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1103,35 +1344,58 @@
                   <a:defRPr/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="sr-Latn-CS" sz="1100" baseline="0"/>
-                  <a:t>Time [%]</a:t>
+                  <a:rPr lang="sr-Latn-CS" sz="1200" baseline="0"/>
+                  <a:t>Time [ms]</a:t>
                 </a:r>
+                <a:endParaRPr lang="en-US" sz="1200" baseline="0"/>
               </a:p>
             </c:rich>
           </c:tx>
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="59521024"/>
+        <c:spPr>
+          <a:noFill/>
+        </c:spPr>
+        <c:crossAx val="125142016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="20"/>
       </c:valAx>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </c:spPr>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="1"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1" i="0" baseline="0"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.78104851207714365"/>
-          <c:y val="8.3215750846157635E-2"/>
-          <c:w val="0.19829036281001661"/>
-          <c:h val="0.14658476001491769"/>
+          <c:x val="0.83015266841644786"/>
+          <c:y val="0.16755043013391041"/>
+          <c:w val="0.1504028871391076"/>
+          <c:h val="0.15488984556817095"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1140,7 +1404,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1200"/>
+            <a:defRPr sz="1200" baseline="0"/>
           </a:pPr>
           <a:endParaRPr lang="en-US"/>
         </a:p>
@@ -1150,9 +1414,14 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+  </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000122" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000122" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1185,248 +1454,7 @@
               <a:rPr lang="sr-Latn-CS" baseline="0">
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>Mutable performance</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" baseline="0">
-              <a:latin typeface="+mn-lt"/>
-            </a:endParaRPr>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.28540755467196821"/>
-          <c:y val="2.5022341376228784E-2"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Mutable!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>integer</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Mutable!$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>test #1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Mutable!$D$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Mutable!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>jodd</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6">
-                <a:lumMod val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Mutable!$A$2</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>test #1</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Mutable!$E$2</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>19.294342021614749</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="75"/>
-        <c:overlap val="40"/>
-        <c:axId val="39584256"/>
-        <c:axId val="39800768"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="39584256"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39800768"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="39800768"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="100"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" vert="horz"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="sr-Latn-CS" sz="1100" baseline="0"/>
-                  <a:t>Time [%]</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="0"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39584256"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-        <c:majorUnit val="20"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.78104851207714365"/>
-          <c:y val="8.3215750846157635E-2"/>
-          <c:w val="0.19829036281001666"/>
-          <c:h val="0.14658476001491769"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="0"/>
-      <c:txPr>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200"/>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000144" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000144" header="0.30000000000000032" footer="0.30000000000000032"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="134"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="34"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr/>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="sr-Latn-CS" baseline="0">
-                <a:latin typeface="+mn-lt"/>
-              </a:rPr>
-              <a:t>Base64 performance</a:t>
+              <a:t>Base64 benchmark</a:t>
             </a:r>
             <a:endParaRPr lang="en-US" baseline="0">
               <a:latin typeface="+mn-lt"/>
@@ -1466,37 +1494,54 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Base64!$C$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>129</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Base64!$C$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>129</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Base64!$A$2:$A$4</c:f>
+              <c:f>Base64!$A$3:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>test #1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>test #2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>test #3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Base64!$F$2:$F$4</c:f>
+              <c:f>Base64!$B$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>100</c:v>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>18650</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1507,7 +1552,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Base64!$C$1</c:f>
+              <c:f>Base64!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1531,37 +1576,54 @@
             </a:ln>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Base64!$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>37</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Base64!$E$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>37</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Base64!$A$2:$A$4</c:f>
+              <c:f>Base64!$A$3:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>test #1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>test #2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>test #3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Base64!$G$2:$G$4</c:f>
+              <c:f>Base64!$D$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>6.6552284630666421</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16.914016489988221</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20.456964450436388</c:v>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2438</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1572,7 +1634,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Base64!$D$1</c:f>
+              <c:f>Base64!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1582,37 +1644,54 @@
             </c:strRef>
           </c:tx>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Base64!$G$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>43</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Base64!$G$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>43</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Base64!$A$2:$A$4</c:f>
+              <c:f>Base64!$A$3:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>test #1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>test #2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>test #3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Base64!$H$2:$H$4</c:f>
+              <c:f>Base64!$F$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>9.2920353982300892</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>21.241797072185765</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>27.825870999787128</c:v>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>3786</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1632,37 +1711,54 @@
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>Base64!$I$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>7</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>Base64!$I$3</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="1"/>
+                  <c:pt idx="0">
+                    <c:v>7</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>Base64!$A$2:$A$4</c:f>
+              <c:f>Base64!$A$3:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="3"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
                   <c:v>test #1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>test #2</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>test #3</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Base64!$I$2:$I$4</c:f>
+              <c:f>Base64!$H$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>1.4719162001083619</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>6.1854282348981995</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>10.029802029376286</c:v>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>962</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1678,11 +1774,11 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="39585792"/>
-        <c:axId val="39803072"/>
+        <c:axId val="42813952"/>
+        <c:axId val="125290176"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="39585792"/>
+        <c:axId val="42813952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1691,7 +1787,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39803072"/>
+        <c:crossAx val="125290176"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1699,10 +1795,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="39803072"/>
+        <c:axId val="125290176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1718,7 +1813,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="sr-Latn-CS" sz="1100" baseline="0"/>
-                  <a:t>Time [%]</a:t>
+                  <a:t>Time [ms]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1730,14 +1825,26 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="39585792"/>
+        <c:crossAx val="42813952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="20"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:legendEntry>
+        <c:idx val="3"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1200" b="1"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+      </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
@@ -1772,7 +1879,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -1799,15 +1906,19 @@
               <a:rPr lang="sr-Latn-CS" baseline="0">
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
-              <a:t>StringBand performance</a:t>
+              <a:t>StringBand benchmark</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US" baseline="0">
-              <a:latin typeface="+mn-lt"/>
-            </a:endParaRPr>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.26742335290280494"/>
+          <c:y val="2.1447721179624665E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1818,7 +1929,7 @@
         <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="3"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
@@ -1826,7 +1937,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>StringBuilder</c:v>
+                  <c:v>String</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1834,41 +1945,86 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>StringBand!$A$2:$A$5</c:f>
+              <c:f>StringBand!$A$3:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>10^2</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>add2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10^3</c:v>
+                  <c:v>add3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10^4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10^5</c:v>
+                  <c:v>add5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>StringBand!$E$2:$E$5</c:f>
+              <c:f>StringBand!$B$3:$B$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1169</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>1371</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>100</c:v>
+                  <c:v>2261</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>StringBand!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>StringBuilder</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>StringBand!$A$3:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>add2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>add3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>add5</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>StringBand!$D$3:$D$5</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>1168</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1371</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2280</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1876,10 +2032,10 @@
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>StringBand!$C$1</c:f>
+              <c:f>StringBand!$F$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1898,94 +2054,35 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>StringBand!$A$2:$A$5</c:f>
+              <c:f>StringBand!$A$3:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>10^2</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>add2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>10^3</c:v>
+                  <c:v>add3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>10^4</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>10^5</c:v>
+                  <c:v>add5</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>StringBand!$F$2:$F$5</c:f>
+              <c:f>StringBand!$F$3:$F$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>562</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>84.705882352941174</c:v>
+                  <c:v>1294</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>71.672354948805463</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>85.761201032136995</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>StringBand!$D$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>StringBand
-(w prediction)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:solidFill>
-                <a:schemeClr val="accent6">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-            </a:ln>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>StringBand!$G$2:$G$5</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>83.529411764705884</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>49.351535836177476</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>83.685198217217931</c:v>
+                  <c:v>2120</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2001,20 +2098,21 @@
         </c:dLbls>
         <c:gapWidth val="75"/>
         <c:overlap val="40"/>
-        <c:axId val="109992448"/>
-        <c:axId val="108865792"/>
+        <c:axId val="125095424"/>
+        <c:axId val="125292480"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="109992448"/>
+        <c:axId val="125095424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="108865792"/>
+        <c:crossAx val="125292480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2022,10 +2120,9 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="108865792"/>
+        <c:axId val="125292480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="100"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2041,7 +2138,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="sr-Latn-CS" sz="1100" baseline="0"/>
-                  <a:t>Time [%]</a:t>
+                  <a:t>Time [ms]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2053,16 +2150,15 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="109992448"/>
+        <c:crossAx val="125095424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
-        <c:majorUnit val="20"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
       <c:legendEntry>
-        <c:idx val="1"/>
+        <c:idx val="2"/>
         <c:txPr>
           <a:bodyPr/>
           <a:lstStyle/>
@@ -2074,27 +2170,14 @@
           </a:p>
         </c:txPr>
       </c:legendEntry>
-      <c:legendEntry>
-        <c:idx val="2"/>
-        <c:txPr>
-          <a:bodyPr/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="1" baseline="0"/>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-      </c:legendEntry>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.75214591326769098"/>
           <c:y val="0.15320456256640858"/>
-          <c:w val="0.2334382174830886"/>
-          <c:h val="0.37541111650587911"/>
+          <c:w val="0.20811978048198521"/>
+          <c:h val="0.21357857611548556"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -2125,16 +2208,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>533399</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>533398</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>523874</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>76198</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2160,20 +2243,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>361950</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>133349</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>495299</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>57150</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>66674</xdr:rowOff>
+      <xdr:rowOff>161924</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="2" name="Chart 1"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2195,16 +2278,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>104774</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2230,20 +2313,20 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>361950</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>133348</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171448</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2265,16 +2348,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>333374</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>409575</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2300,51 +2383,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>333375</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>180974</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>276225</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>485774</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2655,62 +2703,80 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="A1:F3"/>
+      <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" customWidth="1"/>
+    <col min="2" max="3" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>7361</v>
-      </c>
-      <c r="C2">
-        <v>2585</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-      <c r="E2">
-        <f>C2/B2 * 100</f>
-        <v>35.117511207716348</v>
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>2091</v>
+      </c>
+      <c r="C3">
+        <v>23.088000000000001</v>
+      </c>
+      <c r="D3">
+        <v>1058</v>
+      </c>
+      <c r="E3">
+        <v>9.3529999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>20883</v>
-      </c>
-      <c r="C3">
-        <v>7698</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-      <c r="E3">
-        <f>C3/B3 * 100</f>
-        <v>36.862519752909066</v>
+      <c r="B4">
+        <v>6205</v>
+      </c>
+      <c r="C4">
+        <v>86.784000000000006</v>
+      </c>
+      <c r="D4">
+        <v>3083</v>
+      </c>
+      <c r="E4">
+        <v>43.354999999999997</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="0" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2719,157 +2785,206 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="16.42578125" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="6"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2">
-        <v>32655</v>
-      </c>
-      <c r="C2">
-        <v>7982</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-      <c r="E2">
-        <f>C2/B2 * 100</f>
-        <v>24.44342367171949</v>
+      <c r="B2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>813.19399999999996</v>
+      </c>
+      <c r="C3">
+        <v>16.646000000000001</v>
+      </c>
+      <c r="D3">
+        <v>170.78800000000001</v>
+      </c>
+      <c r="E3">
+        <v>23.797000000000001</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>23498</v>
-      </c>
-      <c r="C2">
-        <v>13438</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-      <c r="E2">
-        <f>C2/B2 * 100</f>
-        <v>57.187845774108439</v>
+    <row r="2" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>12260</v>
+      </c>
+      <c r="C3">
+        <v>340</v>
+      </c>
+      <c r="D3">
+        <v>6617</v>
+      </c>
+      <c r="E3">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
-        <v>18891</v>
-      </c>
-      <c r="C3">
-        <v>8800</v>
-      </c>
-      <c r="D3">
-        <v>100</v>
-      </c>
-      <c r="E3">
-        <f>C3/B3 * 100</f>
-        <v>46.583028955587316</v>
+      <c r="B4">
+        <v>8205</v>
+      </c>
+      <c r="C4">
+        <v>385</v>
+      </c>
+      <c r="D4">
+        <v>4092</v>
+      </c>
+      <c r="E4">
+        <v>179</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>7</v>
-      </c>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="6"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>2873</v>
-      </c>
-      <c r="C2">
-        <v>1642</v>
-      </c>
-      <c r="D2">
-        <v>8482</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-      <c r="F2">
-        <f>C2/B2 * 100</f>
-        <v>57.152801949182042</v>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>5594</v>
+      </c>
+      <c r="C3">
+        <v>274</v>
+      </c>
+      <c r="D3">
+        <v>4260</v>
+      </c>
+      <c r="E3">
+        <v>203</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -2877,299 +2992,228 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q12" sqref="Q12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
+      <c r="I1" s="6"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>12584</v>
-      </c>
-      <c r="C2">
-        <v>2428</v>
-      </c>
-      <c r="D2">
-        <v>100</v>
-      </c>
-      <c r="E2">
-        <f>C2/B2 * 100</f>
-        <v>19.294342021614749</v>
+      <c r="B3">
+        <v>18650</v>
+      </c>
+      <c r="C3">
+        <v>129</v>
+      </c>
+      <c r="D3">
+        <v>2438</v>
+      </c>
+      <c r="E3">
+        <v>37</v>
+      </c>
+      <c r="F3">
+        <v>3786</v>
+      </c>
+      <c r="G3">
+        <v>43</v>
+      </c>
+      <c r="H3">
+        <v>962</v>
+      </c>
+      <c r="I3">
+        <v>7</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="0" copies="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>22148</v>
-      </c>
-      <c r="C2">
-        <v>1474</v>
-      </c>
-      <c r="D2">
-        <v>2058</v>
-      </c>
-      <c r="E2">
-        <v>326</v>
-      </c>
-      <c r="F2">
-        <v>100</v>
-      </c>
-      <c r="G2">
-        <f>C2/B2 * 100</f>
-        <v>6.6552284630666421</v>
-      </c>
-      <c r="H2">
-        <f>D2/B2 * 100</f>
-        <v>9.2920353982300892</v>
-      </c>
-      <c r="I2">
-        <f>E2/B2 * 100</f>
-        <v>1.4719162001083619</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>29715</v>
-      </c>
-      <c r="C3">
-        <v>5026</v>
-      </c>
-      <c r="D3">
-        <v>6312</v>
-      </c>
-      <c r="E3">
-        <v>1838</v>
-      </c>
-      <c r="F3">
-        <v>100</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G4" si="0">C3/B3 * 100</f>
-        <v>16.914016489988221</v>
-      </c>
-      <c r="H3">
-        <f t="shared" ref="H3:H4" si="1">D3/B3 * 100</f>
-        <v>21.241797072185765</v>
-      </c>
-      <c r="I3">
-        <f t="shared" ref="I3:I4" si="2">E3/B3 * 100</f>
-        <v>6.1854282348981995</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>28186</v>
-      </c>
-      <c r="C4">
-        <v>5766</v>
-      </c>
-      <c r="D4">
-        <v>7843</v>
-      </c>
-      <c r="E4">
-        <v>2827</v>
-      </c>
-      <c r="F4">
-        <v>100</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="0"/>
-        <v>20.456964450436388</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="1"/>
-        <v>27.825870999787128</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="2"/>
-        <v>10.029802029376286</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="4" max="5" width="14" customWidth="1"/>
+    <col min="6" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="2"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3">
+        <v>1169</v>
+      </c>
+      <c r="C3">
+        <v>34.4</v>
+      </c>
+      <c r="D3">
+        <v>1168</v>
+      </c>
+      <c r="E3">
+        <v>42.3</v>
+      </c>
+      <c r="F3">
+        <v>562</v>
+      </c>
+      <c r="G3">
+        <v>14.8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4">
+        <v>1371</v>
+      </c>
+      <c r="C4">
+        <v>17.399999999999999</v>
+      </c>
+      <c r="D4">
+        <v>1371</v>
+      </c>
+      <c r="E4">
         <v>21</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>22</v>
+      <c r="F4">
+        <v>1294</v>
+      </c>
+      <c r="G4">
+        <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2">
-        <v>9</v>
-      </c>
-      <c r="C2">
-        <v>9</v>
-      </c>
-      <c r="D2">
-        <v>9</v>
-      </c>
-      <c r="E2">
-        <v>100</v>
-      </c>
-      <c r="F2">
-        <f>C2/B2 * 100</f>
-        <v>100</v>
-      </c>
-      <c r="G2">
-        <f>D2/B2 * 100</f>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>19</v>
       </c>
-      <c r="B3">
-        <v>85</v>
-      </c>
-      <c r="C3">
-        <v>72</v>
-      </c>
-      <c r="D3">
-        <v>71</v>
-      </c>
-      <c r="E3">
-        <v>100</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F5" si="0">C3/B3 * 100</f>
-        <v>84.705882352941174</v>
-      </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G5" si="1">D3/B3 * 100</f>
-        <v>83.529411764705884</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4">
-        <v>1465</v>
-      </c>
-      <c r="C4">
-        <v>1050</v>
-      </c>
-      <c r="D4">
-        <v>723</v>
-      </c>
-      <c r="E4">
-        <v>100</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="0"/>
-        <v>71.672354948805463</v>
-      </c>
-      <c r="G4">
-        <f t="shared" si="1"/>
-        <v>49.351535836177476</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>20</v>
-      </c>
       <c r="B5">
-        <v>17052</v>
+        <v>2261</v>
       </c>
       <c r="C5">
-        <v>14624</v>
+        <v>21</v>
       </c>
       <c r="D5">
-        <v>14270</v>
+        <v>2280</v>
       </c>
       <c r="E5">
-        <v>100</v>
+        <v>50.7</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
-        <v>85.761201032136995</v>
+        <v>2120</v>
       </c>
       <c r="G5">
-        <f t="shared" si="1"/>
-        <v>83.685198217217931</v>
+        <v>44.8</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" copies="0" r:id="rId1"/>
   <drawing r:id="rId2"/>

</xml_diff>